<commit_message>
Changed COP for DH geothermal heatpumps
Changed the COP value from 0.6 to 3.0
</commit_message>
<xml_diff>
--- a/cea/databases/CH/assemblies/SUPPLY.xlsx
+++ b/cea/databases/CH/assemblies/SUPPLY.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20399"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luis.santos\Documents\CityEnergyAnalyst\CityEnergyAnalyst\cea\databases\CH\assemblies\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nimathia\Documents\GitHub\CityEnergyAnalyst\CityEnergyAnalyst\cea\databases\CH\assemblies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3821968-9711-4B11-85C3-4FDA7D5D5F1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68ED9172-88B2-478F-A025-9E665100A512}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="993" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="993" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HEATING" sheetId="22" r:id="rId1"/>
@@ -925,8 +925,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1308,7 +1308,7 @@
         <v>19</v>
       </c>
       <c r="E12" s="6">
-        <v>0.6</v>
+        <v>3</v>
       </c>
       <c r="F12" s="6">
         <v>100</v>
@@ -1811,7 +1811,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
fixes master supply new
</commit_message>
<xml_diff>
--- a/cea/databases/CH/assemblies/SUPPLY.xlsx
+++ b/cea/databases/CH/assemblies/SUPPLY.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fonseca/Documents/GitHub/CityEnergyAnalyst/cea/databases/CH/assemblies/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Jimeno/Documents/GitHub/CityEnergyAnalyst/cea/databases/CH/assemblies/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC1937CF-78D3-DA44-B82D-6274BDAF7BDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1637D72A-55AA-B645-B0ED-742DFBD1B680}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37780" yWindow="-6420" windowWidth="24880" windowHeight="12980" tabRatio="993" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9120" yWindow="740" windowWidth="20280" windowHeight="16740" tabRatio="993" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HEATING" sheetId="22" r:id="rId1"/>
@@ -518,10 +518,10 @@
     </xf>
   </cellXfs>
   <cellStyles count="4">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="Normal 2 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
     <cellStyle name="Normal 3" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2198,7 +2198,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA85FBFF-CAF7-3F46-9739-7A82A2DD17E7}">
   <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="135" zoomScaleNormal="135" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="135" zoomScaleNormal="135" workbookViewId="0">
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
@@ -2211,6 +2211,10 @@
     <col min="5" max="5" width="8.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.83203125" customWidth="1"/>
     <col min="7" max="7" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">

</xml_diff>